<commit_message>
updated events calendar with academic events
</commit_message>
<xml_diff>
--- a/src/data/events_template.xlsx
+++ b/src/data/events_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PengOlivia/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F91E1-C2F3-1445-973F-C6D2D37C253F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3B9724-7E70-A845-BDF6-97124AA10809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26120" windowHeight="15680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="277">
   <si>
     <t>Field</t>
   </si>
@@ -808,6 +808,51 @@
   </si>
   <si>
     <t>Carslaw Seminar Room 350</t>
+  </si>
+  <si>
+    <t>Poker Workshop</t>
+  </si>
+  <si>
+    <t>social x academic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crash course in poker ahead of our poker tournament </t>
+  </si>
+  <si>
+    <t>SUDATA, SQT</t>
+  </si>
+  <si>
+    <t>Learn the fundamentals of R programming for data analysis, and connect with new friends in a relaxed, supportive environment</t>
+  </si>
+  <si>
+    <t>Meet The Startups</t>
+  </si>
+  <si>
+    <t>SUDATA, SUSMI, STARTUPLINK, MEDSCISOC</t>
+  </si>
+  <si>
+    <t>Datathon</t>
+  </si>
+  <si>
+    <t>SUDATA, COMM-STEM, SYNCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amstelveen Consulting Workshop </t>
+  </si>
+  <si>
+    <t>Consulting workshop and short case competition practice in collaboration with Amstelveen</t>
+  </si>
+  <si>
+    <t>Data Science Careers Panel</t>
+  </si>
+  <si>
+    <t>SUDATA, 180 Degrees</t>
+  </si>
+  <si>
+    <t>DATA1001/2001 Revision Session</t>
+  </si>
+  <si>
+    <t>STUVAC revision session for DATA1001 and DATA2001 final exam preparation.</t>
   </si>
 </sst>
 </file>
@@ -817,7 +862,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -835,6 +880,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -867,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -880,6 +932,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2729,10 +2784,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2922,6 +2977,238 @@
         <v>40</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="8">
+        <v>46085</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>46087</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B9" s="8">
+        <v>46097</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
+        <v>268</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" s="8">
+        <v>46111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H10" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="8">
+        <v>46132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>272</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="8">
+        <v>46146</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="10">
+        <v>46160</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="10">
+        <v>46174</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" tooltip="https://docs.google.com/forms/d/e/1FAIpQLSeduhevat2fDYJJUjY6mECZbH3QXoC_0hNrDCHVqyYdwnAiqg/viewform?usp=dialog" xr:uid="{B43DCAB3-6C1D-46BC-8239-B038A92F42B4}"/>

</xml_diff>

<commit_message>
fix website pages for phone view
</commit_message>
<xml_diff>
--- a/src/data/events_template.xlsx
+++ b/src/data/events_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PengOlivia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PengOlivia/Desktop/Uni/SUDATA/2026 tech/SUDATA-Website/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3B9724-7E70-A845-BDF6-97124AA10809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA2D85F-11AB-1645-BFC9-2E108CF40473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26120" windowHeight="15680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="26120" windowHeight="15680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="279">
   <si>
     <t>Field</t>
   </si>
@@ -853,6 +853,12 @@
   </si>
   <si>
     <t>STUVAC revision session for DATA1001 and DATA2001 final exam preparation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/forms/d/e/1FAIpQLScgW3fZhxdtB65OgVPNcWrCGxCODn6fjWnh4lLI3cafpXfg_A/viewform </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.google.com/forms/d/e/1FAIpQLScKZVKDVWMbtH2mYJpaJJOdHb3vRpJby2CYVKwQ4UcD3wUGBg/viewform </t>
   </si>
 </sst>
 </file>
@@ -2786,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2886,8 +2892,8 @@
       <c r="H3" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="I3" t="s">
-        <v>40</v>
+      <c r="I3" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -3031,8 +3037,8 @@
       <c r="H8" t="s">
         <v>81</v>
       </c>
-      <c r="I8" t="s">
-        <v>40</v>
+      <c r="I8" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -3212,6 +3218,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" tooltip="https://docs.google.com/forms/d/e/1FAIpQLSeduhevat2fDYJJUjY6mECZbH3QXoC_0hNrDCHVqyYdwnAiqg/viewform?usp=dialog" xr:uid="{B43DCAB3-6C1D-46BC-8239-B038A92F42B4}"/>
+    <hyperlink ref="I8" r:id="rId2" xr:uid="{6CD01B82-3C2B-8F45-8D2A-0AB58BCB324C}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{4159E48D-6FEE-0D4F-9C70-50E56E676DAC}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>